<commit_message>
updade keys mercado pago
</commit_message>
<xml_diff>
--- a/KEYS_EMISSOR.xlsx
+++ b/KEYS_EMISSOR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\Desktop\tratamento-assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44D1244-2BF1-49A3-A1C5-08532B6FFCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40B72B3-728D-4B58-B7B7-F82CB2948B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27795" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27855" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="340">
   <si>
     <t>EMISSOR</t>
   </si>
@@ -1051,6 +1051,9 @@
   </si>
   <si>
     <t>BRDE</t>
+  </si>
+  <si>
+    <t>MERCADO PAGO</t>
   </si>
 </sst>
 </file>
@@ -1430,10 +1433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C195"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1465,7 +1469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1476,7 +1480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1487,7 +1491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1498,7 +1502,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1509,7 +1513,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1520,7 +1524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1531,7 +1535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1542,7 +1546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1553,7 +1557,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1564,7 +1568,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1575,7 +1579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1586,7 +1590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1597,7 +1601,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1608,7 +1612,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1619,7 +1623,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1630,7 +1634,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1641,7 +1645,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1652,7 +1656,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1663,7 +1667,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1674,7 +1678,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1685,7 +1689,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1696,7 +1700,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1707,7 +1711,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1718,7 +1722,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1729,7 +1733,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1740,7 +1744,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1751,7 +1755,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1762,7 +1766,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1773,7 +1777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -1784,7 +1788,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -1795,7 +1799,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -1806,7 +1810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -1817,7 +1821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>61</v>
       </c>
@@ -1828,7 +1832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -1839,7 +1843,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -1850,7 +1854,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -1861,7 +1865,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -1872,7 +1876,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -1883,7 +1887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -1894,7 +1898,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -1905,7 +1909,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -1916,7 +1920,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -1927,7 +1931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -1938,7 +1942,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -1949,7 +1953,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -1960,7 +1964,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>87</v>
       </c>
@@ -1971,7 +1975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>89</v>
       </c>
@@ -1982,7 +1986,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -1993,7 +1997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>93</v>
       </c>
@@ -2004,7 +2008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>95</v>
       </c>
@@ -2015,7 +2019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -2026,7 +2030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>325</v>
       </c>
@@ -2037,7 +2041,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>101</v>
       </c>
@@ -2048,7 +2052,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>103</v>
       </c>
@@ -2059,7 +2063,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>103</v>
       </c>
@@ -2070,7 +2074,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>103</v>
       </c>
@@ -2081,7 +2085,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>107</v>
       </c>
@@ -2092,7 +2096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>325</v>
       </c>
@@ -2103,7 +2107,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>110</v>
       </c>
@@ -2114,7 +2118,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>325</v>
       </c>
@@ -2125,7 +2129,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>113</v>
       </c>
@@ -2136,7 +2140,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>115</v>
       </c>
@@ -2147,7 +2151,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>117</v>
       </c>
@@ -2158,7 +2162,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>120</v>
       </c>
@@ -2169,7 +2173,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>122</v>
       </c>
@@ -2180,7 +2184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>124</v>
       </c>
@@ -2191,7 +2195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>126</v>
       </c>
@@ -2202,7 +2206,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>128</v>
       </c>
@@ -2213,7 +2217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>130</v>
       </c>
@@ -2224,7 +2228,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>132</v>
       </c>
@@ -2235,7 +2239,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>134</v>
       </c>
@@ -2246,7 +2250,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>136</v>
       </c>
@@ -2257,7 +2261,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>136</v>
       </c>
@@ -2268,7 +2272,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>140</v>
       </c>
@@ -2279,7 +2283,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>142</v>
       </c>
@@ -2290,7 +2294,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>144</v>
       </c>
@@ -2301,7 +2305,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>144</v>
       </c>
@@ -2312,7 +2316,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>144</v>
       </c>
@@ -2323,7 +2327,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>148</v>
       </c>
@@ -2334,7 +2338,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>150</v>
       </c>
@@ -2345,7 +2349,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>23</v>
       </c>
@@ -2356,7 +2360,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>138</v>
       </c>
@@ -2367,7 +2371,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>155</v>
       </c>
@@ -2378,7 +2382,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>157</v>
       </c>
@@ -2389,7 +2393,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>158</v>
       </c>
@@ -2400,7 +2404,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>160</v>
       </c>
@@ -2411,7 +2415,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>160</v>
       </c>
@@ -2422,7 +2426,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>160</v>
       </c>
@@ -2433,7 +2437,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>160</v>
       </c>
@@ -2444,7 +2448,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>160</v>
       </c>
@@ -2455,7 +2459,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>160</v>
       </c>
@@ -2466,7 +2470,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>167</v>
       </c>
@@ -2477,7 +2481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>169</v>
       </c>
@@ -2488,7 +2492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>171</v>
       </c>
@@ -2499,7 +2503,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>173</v>
       </c>
@@ -2510,7 +2514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>175</v>
       </c>
@@ -2521,7 +2525,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>175</v>
       </c>
@@ -2532,7 +2536,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>178</v>
       </c>
@@ -2543,7 +2547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>119</v>
       </c>
@@ -2554,7 +2558,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>181</v>
       </c>
@@ -2565,7 +2569,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>183</v>
       </c>
@@ -2576,7 +2580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>183</v>
       </c>
@@ -2587,7 +2591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>185</v>
       </c>
@@ -2598,7 +2602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>186</v>
       </c>
@@ -2609,7 +2613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>328</v>
       </c>
@@ -2620,7 +2624,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>191</v>
       </c>
@@ -2631,7 +2635,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>192</v>
       </c>
@@ -2642,7 +2646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>194</v>
       </c>
@@ -2653,7 +2657,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>196</v>
       </c>
@@ -2664,7 +2668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>198</v>
       </c>
@@ -2675,7 +2679,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>201</v>
       </c>
@@ -2686,7 +2690,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>201</v>
       </c>
@@ -2697,7 +2701,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>204</v>
       </c>
@@ -2708,7 +2712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>206</v>
       </c>
@@ -2719,7 +2723,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>209</v>
       </c>
@@ -2730,7 +2734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>211</v>
       </c>
@@ -2741,7 +2745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>161</v>
       </c>
@@ -2752,7 +2756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>214</v>
       </c>
@@ -2763,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>216</v>
       </c>
@@ -2774,7 +2778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>218</v>
       </c>
@@ -2785,7 +2789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>220</v>
       </c>
@@ -2796,7 +2800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>222</v>
       </c>
@@ -2807,7 +2811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>224</v>
       </c>
@@ -2818,7 +2822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>225</v>
       </c>
@@ -2829,7 +2833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>227</v>
       </c>
@@ -2840,7 +2844,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>230</v>
       </c>
@@ -2851,7 +2855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>232</v>
       </c>
@@ -2862,7 +2866,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>235</v>
       </c>
@@ -2873,7 +2877,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>237</v>
       </c>
@@ -2884,7 +2888,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>239</v>
       </c>
@@ -2895,7 +2899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>241</v>
       </c>
@@ -2906,7 +2910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>243</v>
       </c>
@@ -2917,7 +2921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>245</v>
       </c>
@@ -2928,7 +2932,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>247</v>
       </c>
@@ -2939,7 +2943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>249</v>
       </c>
@@ -2961,7 +2965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>253</v>
       </c>
@@ -2972,7 +2976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>7</v>
       </c>
@@ -2983,7 +2987,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>7</v>
       </c>
@@ -2994,7 +2998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>7</v>
       </c>
@@ -3005,7 +3009,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>7</v>
       </c>
@@ -3016,7 +3020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>7</v>
       </c>
@@ -3027,7 +3031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -3038,7 +3042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>7</v>
       </c>
@@ -3049,7 +3053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>7</v>
       </c>
@@ -3060,7 +3064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>7</v>
       </c>
@@ -3071,7 +3075,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>263</v>
       </c>
@@ -3082,7 +3086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>328</v>
       </c>
@@ -3093,7 +3097,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>266</v>
       </c>
@@ -3104,7 +3108,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>268</v>
       </c>
@@ -3115,7 +3119,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>329</v>
       </c>
@@ -3126,7 +3130,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>329</v>
       </c>
@@ -3137,7 +3141,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>272</v>
       </c>
@@ -3148,7 +3152,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>272</v>
       </c>
@@ -3159,7 +3163,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>272</v>
       </c>
@@ -3170,7 +3174,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>272</v>
       </c>
@@ -3181,7 +3185,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>278</v>
       </c>
@@ -3192,7 +3196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>280</v>
       </c>
@@ -3203,7 +3207,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>283</v>
       </c>
@@ -3214,7 +3218,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>285</v>
       </c>
@@ -3225,7 +3229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>287</v>
       </c>
@@ -3236,7 +3240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>288</v>
       </c>
@@ -3247,7 +3251,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>290</v>
       </c>
@@ -3258,7 +3262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>292</v>
       </c>
@@ -3269,7 +3273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>294</v>
       </c>
@@ -3280,7 +3284,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>296</v>
       </c>
@@ -3291,7 +3295,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>298</v>
       </c>
@@ -3302,7 +3306,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>300</v>
       </c>
@@ -3313,7 +3317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>300</v>
       </c>
@@ -3324,7 +3328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>303</v>
       </c>
@@ -3335,7 +3339,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>305</v>
       </c>
@@ -3346,7 +3350,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>307</v>
       </c>
@@ -3357,7 +3361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>308</v>
       </c>
@@ -3368,7 +3372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>310</v>
       </c>
@@ -3379,7 +3383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>312</v>
       </c>
@@ -3390,7 +3394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>314</v>
       </c>
@@ -3401,7 +3405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>316</v>
       </c>
@@ -3412,7 +3416,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>318</v>
       </c>
@@ -3423,7 +3427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>320</v>
       </c>
@@ -3434,7 +3438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>325</v>
       </c>
@@ -3445,7 +3449,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>323</v>
       </c>
@@ -3456,7 +3460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>329</v>
       </c>
@@ -3467,7 +3471,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>329</v>
       </c>
@@ -3478,7 +3482,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>328</v>
       </c>
@@ -3489,7 +3493,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>328</v>
       </c>
@@ -3500,7 +3504,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>330</v>
       </c>
@@ -3511,7 +3515,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>330</v>
       </c>
@@ -3522,7 +3526,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>330</v>
       </c>
@@ -3533,7 +3537,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>201</v>
       </c>
@@ -3544,7 +3548,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>225</v>
       </c>
@@ -3577,7 +3581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>140</v>
       </c>
@@ -3588,8 +3592,25 @@
         <v>7</v>
       </c>
     </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>251</v>
+      </c>
+      <c r="B196" t="s">
+        <v>339</v>
+      </c>
+      <c r="C196" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C195" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C195" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="MERCADO CRÉDITO SCFI (MERCADO LIVRE)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>